<commit_message>
Avances en el script
</commit_message>
<xml_diff>
--- a/Proyectofinal/SW620_formato_largo.xlsx
+++ b/Proyectofinal/SW620_formato_largo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karol-PC\Desktop\ProyectoFinal-CodigoReproducible\Proyecto final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karol-PC\Desktop\ProyectoFinal-CodigoReproducible\Proyectofinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660A8133-7CB7-4448-A8D2-77CA99559E8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2B036B-997D-4D9E-9FA6-1927AFA6C08C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{320523D2-DF3F-4B3A-99FC-FC2478F3EF45}"/>
   </bookViews>
@@ -51,7 +51,7 @@
     <t>Condicion</t>
   </si>
   <si>
-    <t>Concentracion AntimiRs</t>
+    <t>Concentracion</t>
   </si>
 </sst>
 </file>
@@ -407,15 +407,12 @@
   <dimension ref="A1:T673"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Correccion de todas las observaciones realizadas por la Dra Willink
</commit_message>
<xml_diff>
--- a/Proyectofinal/SW620_formato_largo.xlsx
+++ b/Proyectofinal/SW620_formato_largo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karol-PC\Desktop\ProyectoFinal-CodigoReproducible\Proyectofinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2B036B-997D-4D9E-9FA6-1927AFA6C08C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C156FC56-62C1-4133-947C-8BB2878B9651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{320523D2-DF3F-4B3A-99FC-FC2478F3EF45}"/>
   </bookViews>
@@ -36,22 +36,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t xml:space="preserve">Pseudoreplica </t>
-  </si>
-  <si>
     <t>Tiempo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tratamiento </t>
   </si>
   <si>
     <t>Fluorescencia</t>
   </si>
   <si>
-    <t>Condicion</t>
+    <t>Concentracion</t>
   </si>
   <si>
-    <t>Concentracion</t>
+    <t>Anti-miARNs</t>
+  </si>
+  <si>
+    <t>Recuento_Celular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replicas </t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
   <dimension ref="A1:T673"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,22 +417,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>